<commit_message>
Finished add the first 6 chapters to the excel sheet, which will then be converted into the XML file for chapter generation.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinmorris1/Quarantine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A93AF8D2-53A1-034A-9F2A-63B788352E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{A93AF8D2-53A1-034A-9F2A-63B788352E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{40C02009-95C9-4007-8EB9-173DDD268165}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
   <si>
     <t>chapterId</t>
   </si>
@@ -170,6 +170,294 @@
   </si>
   <si>
     <t>game</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>You're in Leon. (enter apartment) or (enter store) or (go farther)?</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>Leon: Apartment</t>
+  </si>
+  <si>
+    <t>You're in the apartment. (search bedroom) or (leave apartment)?</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Leon: Store</t>
+  </si>
+  <si>
+    <t>You're in the store. (search cabinets) or (leave store)?</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>Leon: Alleyway</t>
+  </si>
+  <si>
+    <t>You're in the alley. (use firecrackers) or (run away)?</t>
+  </si>
+  <si>
+    <t>El Chayote</t>
+  </si>
+  <si>
+    <t>Talk to the farmer. (trade ammo) or (threaten farmer) or (walk away)?</t>
+  </si>
+  <si>
+    <t>Zacatecas</t>
+  </si>
+  <si>
+    <t>You see the town. (go around) or (enter town)?</t>
+  </si>
+  <si>
+    <t>Mountains (East)</t>
+  </si>
+  <si>
+    <t>Prepare for the hike. (drink water) or (eat food) or (use machete) or (start hike)?</t>
+  </si>
+  <si>
+    <t>End of Part 1</t>
+  </si>
+  <si>
+    <t>You have reached the end of Part 1.</t>
+  </si>
+  <si>
+    <t>End of Part 2</t>
+  </si>
+  <si>
+    <t>You have reached the end of Part 2.</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>You have died!</t>
+  </si>
+  <si>
+    <t>Enter Apartment</t>
+  </si>
+  <si>
+    <t>apartment</t>
+  </si>
+  <si>
+    <t>Enter Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter </t>
+  </si>
+  <si>
+    <t>Go Farther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go </t>
+  </si>
+  <si>
+    <t>farther</t>
+  </si>
+  <si>
+    <t>Search Bedroom</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>bedroom</t>
+  </si>
+  <si>
+    <t>pistol ammo,firecrackers</t>
+  </si>
+  <si>
+    <t>Leave Apartment</t>
+  </si>
+  <si>
+    <t>Search Cabinets</t>
+  </si>
+  <si>
+    <t>cabinets</t>
+  </si>
+  <si>
+    <t>Leave Store</t>
+  </si>
+  <si>
+    <t>Use Firecrackers</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>firecrackers</t>
+  </si>
+  <si>
+    <t>Run Away</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>away</t>
+  </si>
+  <si>
+    <t>Trade Ammo</t>
+  </si>
+  <si>
+    <t>Threaten Farmer</t>
+  </si>
+  <si>
+    <t>Walk Away</t>
+  </si>
+  <si>
+    <t>trade</t>
+  </si>
+  <si>
+    <t>ammo</t>
+  </si>
+  <si>
+    <t>pan,medkit</t>
+  </si>
+  <si>
+    <t>threaten</t>
+  </si>
+  <si>
+    <t>farmer</t>
+  </si>
+  <si>
+    <t>pistol,food</t>
+  </si>
+  <si>
+    <t>pistol ammo</t>
+  </si>
+  <si>
+    <t>machete</t>
+  </si>
+  <si>
+    <t>walk</t>
+  </si>
+  <si>
+    <t>Go Around</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>around</t>
+  </si>
+  <si>
+    <t>Enter Town</t>
+  </si>
+  <si>
+    <t>town</t>
+  </si>
+  <si>
+    <t>pocket knife,water</t>
+  </si>
+  <si>
+    <t>water,food</t>
+  </si>
+  <si>
+    <t>Drink Water</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>Eat Food</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>Use Machete</t>
+  </si>
+  <si>
+    <t>Start Hike</t>
+  </si>
+  <si>
+    <t>hike</t>
+  </si>
+  <si>
+    <t>You head towards the store.</t>
+  </si>
+  <si>
+    <t>You turn down Main St and walk out of the city.</t>
+  </si>
+  <si>
+    <t>Inside you find a box of matches and 2L of water. You place them in your backpack, leave the store, and head out of the city.</t>
+  </si>
+  <si>
+    <t>Inside you find a flashlight and a machete. You place them in your backpack, leave the store, and head out of the city.</t>
+  </si>
+  <si>
+    <t>Deciding not to waste any more time, you turn around, leave the store, and head out of the city.</t>
+  </si>
+  <si>
+    <t>You've got water already and would rather not risk unnecessary run-ins, so you turn west and give the city a wide berth.</t>
+  </si>
+  <si>
+    <t>You haven't gotten any water and desperately need a hydration source if you're to continue on your journey. You start walking down the road and into Leon.</t>
+  </si>
+  <si>
+    <t>You crawl through the broken window and into the apartment.</t>
+  </si>
+  <si>
+    <t>You kick down the decrepit door and stumble your way into the store.</t>
+  </si>
+  <si>
+    <t>Nothing looks too interesting, so you decide to continue down the street.</t>
+  </si>
+  <si>
+    <t>You look under the bed and find some pistol ammo and firecrackers. Satisfied with your findings, you leave the bedroom, crawl back out the window, and continue down the street.</t>
+  </si>
+  <si>
+    <t>Pulling open the cabinets, you discover a unopened bottle of water and some food. This should help. After grabbing the items, you head back out of the store and continue down the street.</t>
+  </si>
+  <si>
+    <t>You decide the place looks pretty bare and save time by walking back out and continuing down the street.</t>
+  </si>
+  <si>
+    <t>You decide the place looks pretty bare and save time by crawling back out the window and continuing down the street.</t>
+  </si>
+  <si>
+    <t>You light the firecrackers and throw them over the nearest building. It causes the perfect distraction as you bolt in the opposite direction, keeping to the shadows as you go. Within 20 minutes you are back outside the city.</t>
+  </si>
+  <si>
+    <t>With nothing to distract, you simply run as fast as you can, scrambling and sliding as you go. Someone snatches at your backpack as you blaze by them and a sound follows which sounds oddly like a water bottle hitting the ground… Nevertheless, you make it out of the city alive.</t>
+  </si>
+  <si>
+    <t>Happy with the trade, the farmer happily hands over the frying pan and first aid kit. Nodding your head in thanks, you continue down the dirt road.</t>
+  </si>
+  <si>
+    <t>The farmer cowers in fear, a look of betrayal and sadness in his eyes. You open the chest and find a pistol and some food inside. Greedily you grab them and shove them into your backpack before heading down the dirt road.</t>
+  </si>
+  <si>
+    <t>You politely decline the old farmer's offer and continue down the dirt road.</t>
+  </si>
+  <si>
+    <t>You've got water to spare and no time to waste so you give the city a wide berth and continue on your way.</t>
+  </si>
+  <si>
+    <t>You need some water so you make your way into the city. An overturned truck on one of the roads has a bottle of water and a pocket knife in its remnants. You grab the items and head out of the town.</t>
+  </si>
+  <si>
+    <t>You rest up and drink some water to prepare for the strenuous journey ahead.</t>
+  </si>
+  <si>
+    <t>You rest up and eat some food to prepare for the strenuous journey ahead.</t>
+  </si>
+  <si>
+    <t>Using your machete, you're able to turn a roaming tortoise into a snack. You eat and rest, preparing for the strenuous journey ahead.</t>
+  </si>
+  <si>
+    <t>Ambitously, your begin your journey without any preparation. This is a mistake. Within hours you feel extremely weak and unable to move. Your breath gets harder to catch. As your vision begins to fade you notice several coyotes come out of the bushes and begin to circle you...</t>
   </si>
 </sst>
 </file>
@@ -541,20 +829,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BB1A2F-63DD-CA4F-86FF-FB6F4E825AE5}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -576,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -587,7 +875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -598,7 +886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -609,14 +897,124 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>99</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -628,22 +1026,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA4819E-E7B0-F54E-83C6-1AB902CEB676}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11" style="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
     <col min="6" max="6" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -675,7 +1073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -695,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -714,8 +1112,11 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -734,8 +1135,11 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -757,8 +1161,11 @@
       <c r="G5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -780,8 +1187,11 @@
       <c r="G6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -800,8 +1210,11 @@
       <c r="F7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -818,13 +1231,16 @@
         <v>16</v>
       </c>
       <c r="F8" s="1">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -841,17 +1257,509 @@
         <v>16</v>
       </c>
       <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="J20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="J21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="1">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="1">
+        <v>96</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="1">
+        <v>96</v>
+      </c>
+      <c r="H25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="1">
+      <c r="F26" s="1">
+        <v>96</v>
+      </c>
+      <c r="J26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="1">
+        <v>98</v>
+      </c>
+      <c r="J27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>97</v>
+      </c>
+      <c r="B29" s="1">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>98</v>
+      </c>
+      <c r="B30" s="1">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>99</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B31" s="1">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
resaved .xlsx and .xml files runs locally
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinmorris1/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{A93AF8D2-53A1-034A-9F2A-63B788352E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{40C02009-95C9-4007-8EB9-173DDD268165}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A197999-06AD-5246-B495-B703616E75AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -835,14 +835,14 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
-    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -864,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -875,7 +875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -886,7 +886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -897,7 +897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -908,7 +908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -919,7 +919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -930,7 +930,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -941,7 +941,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -952,7 +952,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -963,7 +963,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -974,7 +974,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>96</v>
       </c>
@@ -985,7 +985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>97</v>
       </c>
@@ -996,7 +996,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>98</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>99</v>
       </c>
@@ -1032,16 +1032,16 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11" style="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>96</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>97</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>98</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Added functionality for use of synonyms by user when inputting commands.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinmorris1/Quarantine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F35202D-97EA-413F-AF5F-D7939775039A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="34380" yWindow="0" windowWidth="17190" windowHeight="21000" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
   <si>
     <t>chapterId</t>
   </si>
@@ -61,9 +61,6 @@
     <t>take</t>
   </si>
   <si>
-    <t>skip</t>
-  </si>
-  <si>
     <t>Enter the Store</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>You're in the store! (take box1) or (take box2) or (leave store)?</t>
   </si>
   <si>
-    <t>You're outside Leon. (skip city) or (enter city)?</t>
-  </si>
-  <si>
     <t>You beat the game! Have a nice day!</t>
   </si>
   <si>
@@ -250,15 +244,9 @@
     <t>Enter Store</t>
   </si>
   <si>
-    <t xml:space="preserve">enter </t>
-  </si>
-  <si>
     <t>Go Farther</t>
   </si>
   <si>
-    <t xml:space="preserve">go </t>
-  </si>
-  <si>
     <t>farther</t>
   </si>
   <si>
@@ -458,6 +446,9 @@
   </si>
   <si>
     <t>Ambitously, your begin your journey without any preparation. This is a mistake. Within hours you feel extremely weak and unable to move. Your breath gets harder to catch. As your vision begins to fade you notice several coyotes come out of the bushes and begin to circle you...</t>
+  </si>
+  <si>
+    <t>You're outside Leon. (go around) or (enter city)?</t>
   </si>
 </sst>
 </file>
@@ -831,18 +822,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BB1A2F-63DD-CA4F-86FF-FB6F4E825AE5}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,18 +844,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -872,150 +863,150 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1028,20 +1019,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA4819E-E7B0-F54E-83C6-1AB902CEB676}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11" style="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
     <col min="6" max="6" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1052,28 +1043,28 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1081,13 +1072,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1102,7 +1093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1110,16 +1101,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>-1</v>
@@ -1131,10 +1122,10 @@
         <v>-1</v>
       </c>
       <c r="J3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1142,13 +1133,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
@@ -1163,30 +1154,30 @@
         <v>-1</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -1195,30 +1186,30 @@
         <v>-1</v>
       </c>
       <c r="J5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -1227,24 +1218,24 @@
         <v>-1</v>
       </c>
       <c r="J6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -1259,10 +1250,10 @@
         <v>-1</v>
       </c>
       <c r="J7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1270,13 +1261,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1288,13 +1279,13 @@
         <v>-1</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1302,13 +1293,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
@@ -1323,10 +1314,10 @@
         <v>-1</v>
       </c>
       <c r="J9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1334,16 +1325,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10">
         <v>-1</v>
@@ -1355,10 +1346,10 @@
         <v>-1</v>
       </c>
       <c r="J10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1366,16 +1357,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11">
         <v>-1</v>
@@ -1387,10 +1378,10 @@
         <v>-1</v>
       </c>
       <c r="J11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1398,16 +1389,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12">
         <v>-1</v>
@@ -1419,30 +1410,30 @@
         <v>-1</v>
       </c>
       <c r="J12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -1451,27 +1442,27 @@
         <v>-1</v>
       </c>
       <c r="J13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G14">
         <v>-1</v>
@@ -1483,30 +1474,30 @@
         <v>-1</v>
       </c>
       <c r="J14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -1515,27 +1506,27 @@
         <v>-1</v>
       </c>
       <c r="J15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G16">
         <v>-1</v>
@@ -1547,24 +1538,24 @@
         <v>-1</v>
       </c>
       <c r="J16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
@@ -1573,30 +1564,30 @@
         <v>-1</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F18" s="1">
         <v>4</v>
@@ -1611,10 +1602,10 @@
         <v>-1</v>
       </c>
       <c r="J18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1622,31 +1613,31 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
         <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" t="s">
-        <v>93</v>
       </c>
       <c r="F19" s="1">
         <v>5</v>
       </c>
       <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19">
+        <v>-1</v>
+      </c>
+      <c r="I19" t="s">
         <v>94</v>
       </c>
-      <c r="H19">
-        <v>-1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>98</v>
-      </c>
       <c r="J19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1654,31 +1645,31 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F20" s="1">
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H20">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1686,13 +1677,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F21" s="1">
         <v>5</v>
@@ -1707,10 +1698,10 @@
         <v>-1</v>
       </c>
       <c r="J21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1718,13 +1709,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F22" s="1">
         <v>6</v>
@@ -1736,13 +1727,13 @@
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1750,19 +1741,19 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F23" s="1">
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -1771,10 +1762,10 @@
         <v>-1</v>
       </c>
       <c r="J23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1782,13 +1773,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" s="1">
         <v>96</v>
@@ -1797,16 +1788,16 @@
         <v>-1</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1814,13 +1805,13 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F25" s="1">
         <v>96</v>
@@ -1829,16 +1820,16 @@
         <v>-1</v>
       </c>
       <c r="H25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1846,13 +1837,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F26" s="1">
         <v>96</v>
@@ -1867,10 +1858,10 @@
         <v>-1</v>
       </c>
       <c r="J26" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1878,13 +1869,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F27" s="1">
         <v>98</v>
@@ -1899,10 +1890,10 @@
         <v>-1</v>
       </c>
       <c r="J27" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>96</v>
       </c>
@@ -1910,7 +1901,7 @@
         <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -1934,7 +1925,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>97</v>
       </c>
@@ -1942,7 +1933,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>-1</v>
@@ -1966,7 +1957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>98</v>
       </c>
@@ -1974,7 +1965,7 @@
         <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -1998,7 +1989,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>99</v>
       </c>
@@ -2006,7 +1997,7 @@
         <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>-1</v>

</xml_diff>

<commit_message>
Added a couple extra synonyms.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F35202D-97EA-413F-AF5F-D7939775039A}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9392A323-01CE-40BB-AB09-952B0A09DF39}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="0" windowWidth="17190" windowHeight="21000" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="3120" yWindow="600" windowWidth="17190" windowHeight="21000" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
     <sheet name="Paths" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,21 +92,6 @@
     <t>loseItems</t>
   </si>
   <si>
-    <t>MC Store</t>
-  </si>
-  <si>
-    <t>Take Box 1</t>
-  </si>
-  <si>
-    <t>box1</t>
-  </si>
-  <si>
-    <t>Take Box 2</t>
-  </si>
-  <si>
-    <t>box2</t>
-  </si>
-  <si>
     <t>Leave the Store</t>
   </si>
   <si>
@@ -148,18 +134,9 @@
     <t>flashlight,machete</t>
   </si>
   <si>
-    <t>You're in Mexico City! (enter store) or (leave city)?</t>
-  </si>
-  <si>
-    <t>You're in the store! (take box1) or (take box2) or (leave store)?</t>
-  </si>
-  <si>
     <t>You beat the game! Have a nice day!</t>
   </si>
   <si>
-    <t>Welcome to our game! (start game)</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -449,15 +426,46 @@
   </si>
   <si>
     <t>You're outside Leon. (go around) or (enter city)?</t>
+  </si>
+  <si>
+    <t>Quest for the Quarantine follows our protagonist, 16-year-old Esperanza, as she navigates post-apocalyptic Mexico in hopes of reaching salvation in the form of the "Quarantine Zone". As we follow Esperanza through her journey, we discover that the most pressing danger is the loss of humanity itself...\n\nWelcome to Quest for the Quarantine! Throughout this playable story you, the player, can enter commands to help Esperanza navigate both her paths and decisions. To begin the game, enter “start game” in the text box below. May you guide Esperanza safely to the Quarantine.</t>
+  </si>
+  <si>
+    <t>In the weeks following The Event, the days were unsafe. She had learned that lesson the hard way with the death of Mama. They took refuge in the night, and for months everything was okay. They even met others who had not succumbed, who were not Violent. They shared stories of past lives, better lives, and hope for salvation. Rumors of a safe zone in the United States, just outside San Diego, persisted among survivors. For a time, they had hope. But slowly, the survivors disappeared, Mama included; so she decided to leave, to seek out the refuge of the quarantine in the States.\n\nShe slipped quietly into the night and made her way through the streets of Mexico City, careful to avoid others. As she approaches the main avenue, she notices a small store along the road heading out of the city. Perhaps I should look for supplies? She ponders. Or is it better to just leave the city?</t>
+  </si>
+  <si>
+    <t>The sign above the door reads “Construcentro”. Esperanza steps through the shadowed doorframe and is immediately hit with the smell of mildew. She gazes around the dark store- and notes it’s pretty barren. To her right along the wall is an old storage crate and behind the counter is an unopened delivery box. Outside, some distant shouting appears to grow stronger. If she’s going to grab something, she should be quick.</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>crate</t>
+  </si>
+  <si>
+    <t>Take Box</t>
+  </si>
+  <si>
+    <t>Take Crate</t>
+  </si>
+  <si>
+    <t>Mexico City: Construcentro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -471,6 +479,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -498,13 +513,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +844,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -849,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,8 +883,8 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
+      <c r="C3" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +892,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
+        <v>137</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +903,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,43 +914,43 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +958,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,10 +969,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,10 +980,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,10 +991,10 @@
         <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,10 +1002,10 @@
         <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,10 +1013,10 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,15 +1024,16 @@
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1020,7 +1042,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1043,10 +1065,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -1061,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1072,13 +1094,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1122,7 +1144,7 @@
         <v>-1</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1154,7 +1176,7 @@
         <v>-1</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1165,19 +1187,19 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -1186,7 +1208,7 @@
         <v>-1</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1197,19 +1219,19 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -1218,7 +1240,7 @@
         <v>-1</v>
       </c>
       <c r="J6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1229,7 +1251,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1250,7 +1272,7 @@
         <v>-1</v>
       </c>
       <c r="J7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1261,13 +1283,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1279,10 +1301,10 @@
         <v>-1</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1293,7 +1315,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1314,7 +1336,7 @@
         <v>-1</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1325,16 +1347,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G10">
         <v>-1</v>
@@ -1346,7 +1368,7 @@
         <v>-1</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1357,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1366,7 +1388,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G11">
         <v>-1</v>
@@ -1378,7 +1400,7 @@
         <v>-1</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1389,16 +1411,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <v>-1</v>
@@ -1410,7 +1432,7 @@
         <v>-1</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1418,22 +1440,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -1442,7 +1464,7 @@
         <v>-1</v>
       </c>
       <c r="J13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1450,19 +1472,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G14">
         <v>-1</v>
@@ -1474,7 +1496,7 @@
         <v>-1</v>
       </c>
       <c r="J14" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1482,22 +1504,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -1506,7 +1528,7 @@
         <v>-1</v>
       </c>
       <c r="J15" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1514,10 +1536,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1526,7 +1548,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G16">
         <v>-1</v>
@@ -1538,7 +1560,7 @@
         <v>-1</v>
       </c>
       <c r="J16" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1546,16 +1568,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
@@ -1564,13 +1586,13 @@
         <v>-1</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1578,16 +1600,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F18" s="1">
         <v>4</v>
@@ -1602,7 +1624,7 @@
         <v>-1</v>
       </c>
       <c r="J18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1613,28 +1635,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F19" s="1">
         <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H19">
         <v>-1</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1645,28 +1667,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F20" s="1">
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H20">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1677,13 +1699,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F21" s="1">
         <v>5</v>
@@ -1698,7 +1720,7 @@
         <v>-1</v>
       </c>
       <c r="J21" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1709,13 +1731,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1">
         <v>6</v>
@@ -1727,10 +1749,10 @@
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J22" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1741,19 +1763,19 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1">
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -1762,7 +1784,7 @@
         <v>-1</v>
       </c>
       <c r="J23" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1773,13 +1795,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>96</v>
@@ -1788,13 +1810,13 @@
         <v>-1</v>
       </c>
       <c r="H24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1805,13 +1827,13 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F25" s="1">
         <v>96</v>
@@ -1820,13 +1842,13 @@
         <v>-1</v>
       </c>
       <c r="H25" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I25" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1837,13 +1859,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1">
         <v>96</v>
@@ -1858,7 +1880,7 @@
         <v>-1</v>
       </c>
       <c r="J26" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1869,13 +1891,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1">
         <v>98</v>
@@ -1890,7 +1912,7 @@
         <v>-1</v>
       </c>
       <c r="J27" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1901,7 +1923,7 @@
         <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -1933,7 +1955,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D29">
         <v>-1</v>
@@ -1965,7 +1987,7 @@
         <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -1997,7 +2019,7 @@
         <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D31">
         <v>-1</v>

</xml_diff>

<commit_message>
Added descriptive story text to excel file.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9392A323-01CE-40BB-AB09-952B0A09DF39}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D532639A-B7F6-4AFA-A48B-333D5AA64D40}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="600" windowWidth="17190" windowHeight="21000" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="34380" yWindow="0" windowWidth="17190" windowHeight="21000" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
     <sheet name="Paths" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="139">
   <si>
     <t>chapterId</t>
   </si>
@@ -110,9 +109,6 @@
     <t>Go Around Leon</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
@@ -134,9 +130,6 @@
     <t>flashlight,machete</t>
   </si>
   <si>
-    <t>You beat the game! Have a nice day!</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -146,72 +139,36 @@
     <t>Leon</t>
   </si>
   <si>
-    <t>You're in Leon. (enter apartment) or (enter store) or (go farther)?</t>
-  </si>
-  <si>
     <t>3A</t>
   </si>
   <si>
     <t>Leon: Apartment</t>
   </si>
   <si>
-    <t>You're in the apartment. (search bedroom) or (leave apartment)?</t>
-  </si>
-  <si>
     <t>3B</t>
   </si>
   <si>
-    <t>Leon: Store</t>
-  </si>
-  <si>
-    <t>You're in the store. (search cabinets) or (leave store)?</t>
-  </si>
-  <si>
     <t>3C</t>
   </si>
   <si>
     <t>Leon: Alleyway</t>
   </si>
   <si>
-    <t>You're in the alley. (use firecrackers) or (run away)?</t>
-  </si>
-  <si>
     <t>El Chayote</t>
   </si>
   <si>
-    <t>Talk to the farmer. (trade ammo) or (threaten farmer) or (walk away)?</t>
-  </si>
-  <si>
     <t>Zacatecas</t>
   </si>
   <si>
-    <t>You see the town. (go around) or (enter town)?</t>
-  </si>
-  <si>
-    <t>Mountains (East)</t>
-  </si>
-  <si>
-    <t>Prepare for the hike. (drink water) or (eat food) or (use machete) or (start hike)?</t>
-  </si>
-  <si>
     <t>End of Part 1</t>
   </si>
   <si>
-    <t>You have reached the end of Part 1.</t>
-  </si>
-  <si>
     <t>End of Part 2</t>
   </si>
   <si>
-    <t>You have reached the end of Part 2.</t>
-  </si>
-  <si>
     <t>Death</t>
   </si>
   <si>
-    <t>You have died!</t>
-  </si>
-  <si>
     <t>Enter Apartment</t>
   </si>
   <si>
@@ -320,9 +277,6 @@
     <t>town</t>
   </si>
   <si>
-    <t>pocket knife,water</t>
-  </si>
-  <si>
     <t>water,food</t>
   </si>
   <si>
@@ -350,84 +304,6 @@
     <t>hike</t>
   </si>
   <si>
-    <t>You head towards the store.</t>
-  </si>
-  <si>
-    <t>You turn down Main St and walk out of the city.</t>
-  </si>
-  <si>
-    <t>Inside you find a box of matches and 2L of water. You place them in your backpack, leave the store, and head out of the city.</t>
-  </si>
-  <si>
-    <t>Inside you find a flashlight and a machete. You place them in your backpack, leave the store, and head out of the city.</t>
-  </si>
-  <si>
-    <t>Deciding not to waste any more time, you turn around, leave the store, and head out of the city.</t>
-  </si>
-  <si>
-    <t>You've got water already and would rather not risk unnecessary run-ins, so you turn west and give the city a wide berth.</t>
-  </si>
-  <si>
-    <t>You haven't gotten any water and desperately need a hydration source if you're to continue on your journey. You start walking down the road and into Leon.</t>
-  </si>
-  <si>
-    <t>You crawl through the broken window and into the apartment.</t>
-  </si>
-  <si>
-    <t>You kick down the decrepit door and stumble your way into the store.</t>
-  </si>
-  <si>
-    <t>Nothing looks too interesting, so you decide to continue down the street.</t>
-  </si>
-  <si>
-    <t>You look under the bed and find some pistol ammo and firecrackers. Satisfied with your findings, you leave the bedroom, crawl back out the window, and continue down the street.</t>
-  </si>
-  <si>
-    <t>Pulling open the cabinets, you discover a unopened bottle of water and some food. This should help. After grabbing the items, you head back out of the store and continue down the street.</t>
-  </si>
-  <si>
-    <t>You decide the place looks pretty bare and save time by walking back out and continuing down the street.</t>
-  </si>
-  <si>
-    <t>You decide the place looks pretty bare and save time by crawling back out the window and continuing down the street.</t>
-  </si>
-  <si>
-    <t>You light the firecrackers and throw them over the nearest building. It causes the perfect distraction as you bolt in the opposite direction, keeping to the shadows as you go. Within 20 minutes you are back outside the city.</t>
-  </si>
-  <si>
-    <t>With nothing to distract, you simply run as fast as you can, scrambling and sliding as you go. Someone snatches at your backpack as you blaze by them and a sound follows which sounds oddly like a water bottle hitting the ground… Nevertheless, you make it out of the city alive.</t>
-  </si>
-  <si>
-    <t>Happy with the trade, the farmer happily hands over the frying pan and first aid kit. Nodding your head in thanks, you continue down the dirt road.</t>
-  </si>
-  <si>
-    <t>The farmer cowers in fear, a look of betrayal and sadness in his eyes. You open the chest and find a pistol and some food inside. Greedily you grab them and shove them into your backpack before heading down the dirt road.</t>
-  </si>
-  <si>
-    <t>You politely decline the old farmer's offer and continue down the dirt road.</t>
-  </si>
-  <si>
-    <t>You've got water to spare and no time to waste so you give the city a wide berth and continue on your way.</t>
-  </si>
-  <si>
-    <t>You need some water so you make your way into the city. An overturned truck on one of the roads has a bottle of water and a pocket knife in its remnants. You grab the items and head out of the town.</t>
-  </si>
-  <si>
-    <t>You rest up and drink some water to prepare for the strenuous journey ahead.</t>
-  </si>
-  <si>
-    <t>You rest up and eat some food to prepare for the strenuous journey ahead.</t>
-  </si>
-  <si>
-    <t>Using your machete, you're able to turn a roaming tortoise into a snack. You eat and rest, preparing for the strenuous journey ahead.</t>
-  </si>
-  <si>
-    <t>Ambitously, your begin your journey without any preparation. This is a mistake. Within hours you feel extremely weak and unable to move. Your breath gets harder to catch. As your vision begins to fade you notice several coyotes come out of the bushes and begin to circle you...</t>
-  </si>
-  <si>
-    <t>You're outside Leon. (go around) or (enter city)?</t>
-  </si>
-  <si>
     <t>Quest for the Quarantine follows our protagonist, 16-year-old Esperanza, as she navigates post-apocalyptic Mexico in hopes of reaching salvation in the form of the "Quarantine Zone". As we follow Esperanza through her journey, we discover that the most pressing danger is the loss of humanity itself...\n\nWelcome to Quest for the Quarantine! Throughout this playable story you, the player, can enter commands to help Esperanza navigate both her paths and decisions. To begin the game, enter “start game” in the text box below. May you guide Esperanza safely to the Quarantine.</t>
   </si>
   <si>
@@ -450,15 +326,205 @@
   </si>
   <si>
     <t>Mexico City: Construcentro</t>
+  </si>
+  <si>
+    <t>It has been nearly two relatively uneventful weeks since Esperanza has departed Mexico City. After roughly 500 km of hiking, her feet hurt, and she is beginning to run low on supplies. On the twelfth day of her journey, she crests a ridge and spots a city in the valley below. Judging by the nearby highway sign, it’s the city of Leon. The sun is beginning to set behind her, and she notes several light sources dotting the city’s landscape- there’s people there, potentially dangerous people. On one hand, she needs to make a supply run, but on the other she really likes being alive. She could possibly give the city a wide berth, ignoring it completely, but only if she has enough water in her backpack.</t>
+  </si>
+  <si>
+    <t>The sun has now fully disappeared behind the horizon as she makes her way into Leon. Old, decrepit cars accentuate the crumbling roadways, abundant with unregulated vegetation. There are definite signs of habitation however, as she notes some uncorroded ammunition shells at the entry of an alleyway. She pauses to look back and reconsider her decision, but eventually decides to continue forward. An hour later she enters a small square overlooking a dry fountain. A dull glow illuminates the city skyline to her right, giving her pause. The time to search is now, she decides, not wanting to risk spending any more time in the city. She gazes around the square and notes a couple potential looting points: an apartment across the square with a shattered second-story window and a fire escape, and a small bodega below with a very rusted wrought-iron door that seems to be barely hanging on. Additionally, she could continue farther down the road.</t>
+  </si>
+  <si>
+    <t>Leon: Bodega</t>
+  </si>
+  <si>
+    <r>
+      <t>Once inside the apartment, Esperanza immediately regrets her decision. A violent smell assaults her nose…</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">something is dead in here. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With her senses heightened, Esperanza peers down the hallway and notices two doors: one open and one closed. It’s evident the smell is coming from the closed door, but with a quick glance the other room appears to be a bedroom. With her back to the closed door, the hair on her neck begins to stand. She notices a faint, rhythmic creaking coming from the closed room. Between the smell and the adrenaline, she considers escaping the apartment as fast as possible. But there may be treasure to be had within the bedroom.</t>
+    </r>
+  </si>
+  <si>
+    <t>bodega</t>
+  </si>
+  <si>
+    <t>The bodega is dimly lit, and it appears to Esperanza that she is far from being the first person to scavenge in here. Empty bottles and wrappers layer the floor. Few things remain untouched. She picks her way around the discarded remnants for a while, but it proves unfruitful. A distant sound, possibly human, cause her to bolt upright, eyes wide. She cocks her head and listens for a while but notices no other sounds. As she makes her way to the doorway, she notices a small cabinet with closed doors behind the counter. It’s low to the ground and otherwise hidden at eye level.</t>
+  </si>
+  <si>
+    <t>As Esperanza is making her way out of the city, she can’t help but shake the feeling that someone is watching her. She pauses in the dark and searches the shadows for a sign of movement. Nothing. She continues walking, but the process repeats itself at least a dozen more times. And then there’s the noise: a faint jingle, like that of a glass bottle rolling on concrete. Time slows down and she feels every muscle in her body tighten like a loaded spring. She releases and within two steps, the sound of whoops and shouts light up the concrete jungle. She can hear several sets of footsteps behind her in the dark. She sprints- ducking around corners and dodging between cars. After several minutes, she begins to grow tired and the voices more distant. In a dark alley she pauses, catching her breath. It’s make or break time. She estimates that she’s about 5 minutes from the city limits. Can she use something as a distraction perhaps? She thinks she can make the run, but it sure would help to divert their attention. Either way, she needs to get out of the city immediately.</t>
+  </si>
+  <si>
+    <t>A week later, Esperanza finds herself trudging along a dirt road in the midday heat. A nearby sign points back the way she came and reads “El Chayote – 20 km”. Since Leon, she had played it safe and avoided any large settlements. No need to press my luck, she thinks to herself. As she comes around a bend in the road, she notices a small farmstead to her right. The remnants of a fenced pasture dot the roadside, but there is no livestock to be seen. A small dirt path winds from the road back several hundred meters to a house. At the end of the path is a wooden chair, and in that chair, an elderly man. He nods to Esperanza as she approaches, and she regards him cautiously. After some small discussion, the farmer attempts to initiate a barter. He wants any ammunition she may have and he’s offering the contents of a medium-sized sack he has laying on the ground next to his chair and a small, wooden box.</t>
+  </si>
+  <si>
+    <t>Quest for the Quarantine</t>
+  </si>
+  <si>
+    <t>At long last Esperanza reaches the base of the mountains known as the Sierra Madre. She rests for a day before starting her journey. It would benefit her to get some sustenance before the next leg of her journey. Perhaps some food or water, or she could even hunt if she had the right tools.</t>
+  </si>
+  <si>
+    <t>Sierra Madre Foothills (East)</t>
+  </si>
+  <si>
+    <t>You have reached the end of Part 1 of Esperanza’s story. We hope to have Parts 2 and 3 ready in the near future. Thank you for guiding Esperanza on her journey!</t>
+  </si>
+  <si>
+    <t>Esperanza has died. You make a terrible guide. Feel free to start over and uh…try not get her killed again.</t>
+  </si>
+  <si>
+    <t>You have reached the end of Part 1 of Esperanza’s story. We hope to have Part 3 ready in the near future. Thank you for guiding Esperanza on her journey!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Esperanza has successfully completed her journey and she thanks you for guiding her to safety. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+  </si>
+  <si>
+    <t>Esperanza decides the smartest thing to do is to look for some supplies before her trek and makes her way towards the store.</t>
+  </si>
+  <si>
+    <t>No need to waste any more time in this god-forsaken city. Esperanza disregards the small store and continues down the main road and out of the city.</t>
+  </si>
+  <si>
+    <t>She decides the box looks more promising and quickly makes her way over to it. A quick pull rips through the tape and exposes the contents inside: a box of matches and 2L of water. Not too bad. She grabs the items and places them in her backpack before turning and heading back out the door, and out of the city.</t>
+  </si>
+  <si>
+    <t>She decides the crate looks more promising and quickly makes her way over to it. Peering inside, she finds two items: a flashlight and a machete. Not too bad. She grabs the items and places them in her backpack before turning and heading back out the door, and out of the city.</t>
+  </si>
+  <si>
+    <t>She decides the best course of action is to just get out of the city as soon as possible. Heading back out the door of Construcentro, she continues down the main road and out of the city.</t>
+  </si>
+  <si>
+    <t>She’s got enough water and would rather not risk unnecessary contact with individuals, so she decides to go around the city and avoid it completely. She heads down the ridge and sticks to the west, keeping several kilometers between her and the urban center.</t>
+  </si>
+  <si>
+    <t>She really needs some more water and after two weeks on the road, some additional supplies wouldn’t hurt either. She heads down the ridge and makes her way into the city.</t>
+  </si>
+  <si>
+    <t>Being on the second story, the apartment is less likely to be picked clean, she reasons. She approaches the fire escape and winces at every creak as she scrambles up it. Once at the top, she carefully makes her way across the broken glass and through the window frame.</t>
+  </si>
+  <si>
+    <t>Noting the distant lights and likely nearby danger, she decides to keep to the ground for a quick escape. She approaches the bodega and surveys the door before grasping it with both hands and simply ripping it off. It’s heavier than she expects and clatters to the ground, making her wince at the exposure. Pausing for a minute, she shuffles through the doorway and into the dark.</t>
+  </si>
+  <si>
+    <t>Nothing looks overly promising, so she keeps winding her way through the rubble and down the street.</t>
+  </si>
+  <si>
+    <t>The fear is too great, and rightly so. She turns and quickly tiptoes back out of the window and down the fire escape.</t>
+  </si>
+  <si>
+    <r>
+      <t>Risk versus reward…. the potential reward is quite tempting. Taking a deep breath, she steps into the bedroom and begins searching. The last place she checks is under the bed: a small wooden keepsake box resides there. She opens it and her eyes grow wide at the sight of some pistol ammunition and a string of firecrackers. Excitedly she shoves them in her pockets and rushes out of the room. A previously unseen wet spot causes her to slip and fall backwards into the closed door, forcing it open. She lands on her butt with her back against a solid piece of furniture. The smell is overwhelming now, and she immediately squints her eyes and vomits. Sitting back up, she notices a faint brushing against her cheek. She is paralyzed in fear but manages to look out of the corner of her eye. Toes</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Someone’s toes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are rubbing against her cheek, suspended from above. Not daring to look up, she crawls on all fours out of the new room and scrambles to get out of the apartment and out of this city.</t>
+    </r>
+  </si>
+  <si>
+    <t>She pulls open the cabinet doors and hurriedly searches, grasping a bottle of water and a small packet of food. Good enough for me, she concludes, before turning and leaving the store.</t>
+  </si>
+  <si>
+    <t>The sound has her spooked and she decides to just get away from the square with haste. She steps out of the store and keeps winding her way through the rubble and down the street.</t>
+  </si>
+  <si>
+    <t>Pulling the firecrackers out of her pocket, she quickly lights them and lobs them over the roof of the building behind her. She pivots 180 degrees and immediately sprints down the roadway. Behind her the sounds of cracks, snaps, and pops greet her, followed by a delayed shouting. She grins assuredly (success!) and is out of the city limits within a few minutes.</t>
+  </si>
+  <si>
+    <t>Mistakenly she immediately runs out of the alley and into a shadowy figure, both falling to the ground. She scrambles to her feet, but the person has a hand on her backpack. Digging her heels in, she pulls forward and a small ripping sound issues from her backpack. The person falls to the ground again and the sound of something falling out of her backpack fills the night. No time. She sprints with every ounce of energy she can muster and is out of the city in minutes, alone and safe.</t>
+  </si>
+  <si>
+    <t>Esperanza acquiesces and holds out her ammo. The farmer looks excited and hands her the sack in return, which she then opens and peers inside. The contents are a small first aid kit and a cooking pan; they could prove useful. She throws the sack over her shoulder, waves goodbye, and continues down the dirt road.</t>
+  </si>
+  <si>
+    <t>Esperanza whips out her machete and raises it in the air menacingly. Surprised, the farmer stumbles backwards, a look of betrayal in his eyes. She tells him to run and he doesn’t hesitate, bounding back towards the house with the sack in his hand. She readies to follow him but notices the wooden box on the ground. Opening it, she finds a pistol and some food. Deciding that’s enough of a procurement, she let’s the farmer live another day.</t>
+  </si>
+  <si>
+    <t>She politely declines the farmer’s offer and wishes him well. It’s a relief to meet someone not Violent, she thinks to herself as she continues down the dirt road. Something that seems to be happening less frequently as time wears on.</t>
+  </si>
+  <si>
+    <t>As Esperanza’s odyssey continues, the mountains in the distance continue to grow larger. She knows the time is getting near for her to traverse the range and reach the western side. As she reaches the foothills, a small village lies in her path. At first observation, it seems completely abandoned. This might be her last chance to get supplies before she summits, but it isn’t devoid of risk. She would need water if she were going to go around the town.</t>
+  </si>
+  <si>
+    <t>pocketknife,water</t>
+  </si>
+  <si>
+    <t>She has water to spare and no time to waste, so she gives the village a wide berth and continues on her way.</t>
+  </si>
+  <si>
+    <t>She walks down the small main road and into the village. The place is devoid of any signs of life, a sadly reassuring attribute to Esperanza. Towards the center of the village, she finds an overturned truck with its contents and broken glass strewn about. She rummages about and is able to acquire a pocketknife in quite good condition and another bottle of water. Satisfied, she follows the road out of the village.</t>
+  </si>
+  <si>
+    <t>Hydrate or die-drate, she muses. She downs another liter of water, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>A rumbling stomach concludes that she needs to eat. She downs another packet of food, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>Using her machete, she’s able to turn a roaming tortoise into a solid meal. She eats, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>Ambitiously, she immediately begins the hike into the mountains. Within hours she feels extremely weak and can barely move. Her muscles tighten and cramp with every passing moment. Her breath gets harder to catch, the panting is never-ending. Her vision slowly begins to fade, but not before she notices several moving shapes around her. Coyotes are circling her. A sharp pain followed by warmth. And then darkness.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -492,6 +558,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Emoji"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -513,15 +593,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -843,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BB1A2F-63DD-CA4F-86FF-FB6F4E825AE5}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -870,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +967,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,10 +975,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -905,8 +988,8 @@
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>129</v>
+      <c r="C5" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,43 +997,43 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
+        <v>99</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,10 +1052,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,10 +1063,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
+        <v>107</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +1074,10 @@
         <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,10 +1085,10 @@
         <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,25 +1096,25 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1041,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA4819E-E7B0-F54E-83C6-1AB902CEB676}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1065,10 +1148,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -1094,13 +1177,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1143,8 +1226,8 @@
       <c r="I3">
         <v>-1</v>
       </c>
-      <c r="J3" t="s">
-        <v>104</v>
+      <c r="J3" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1175,8 +1258,8 @@
       <c r="I4">
         <v>-1</v>
       </c>
-      <c r="J4" t="s">
-        <v>105</v>
+      <c r="J4" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1187,19 +1270,19 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -1207,8 +1290,8 @@
       <c r="I5">
         <v>-1</v>
       </c>
-      <c r="J5" t="s">
-        <v>106</v>
+      <c r="J5" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1219,19 +1302,19 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -1239,8 +1322,8 @@
       <c r="I6">
         <v>-1</v>
       </c>
-      <c r="J6" t="s">
-        <v>107</v>
+      <c r="J6" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1271,8 +1354,8 @@
       <c r="I7">
         <v>-1</v>
       </c>
-      <c r="J7" t="s">
-        <v>108</v>
+      <c r="J7" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1286,10 +1369,10 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1297,14 +1380,14 @@
       <c r="G8">
         <v>-1</v>
       </c>
-      <c r="H8">
-        <v>-1</v>
+      <c r="H8" t="s">
+        <v>21</v>
       </c>
       <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" t="s">
-        <v>109</v>
+      <c r="J8" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1335,8 +1418,8 @@
       <c r="I9">
         <v>-1</v>
       </c>
-      <c r="J9" t="s">
-        <v>110</v>
+      <c r="J9" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,16 +1430,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G10">
         <v>-1</v>
@@ -1367,8 +1450,8 @@
       <c r="I10">
         <v>-1</v>
       </c>
-      <c r="J10" t="s">
-        <v>111</v>
+      <c r="J10" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,16 +1462,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <v>-1</v>
@@ -1399,8 +1482,8 @@
       <c r="I11">
         <v>-1</v>
       </c>
-      <c r="J11" t="s">
-        <v>112</v>
+      <c r="J11" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1411,16 +1494,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G12">
         <v>-1</v>
@@ -1431,8 +1514,8 @@
       <c r="I12">
         <v>-1</v>
       </c>
-      <c r="J12" t="s">
-        <v>113</v>
+      <c r="J12" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1440,22 +1523,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -1463,8 +1546,8 @@
       <c r="I13">
         <v>-1</v>
       </c>
-      <c r="J13" t="s">
-        <v>114</v>
+      <c r="J13" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1472,19 +1555,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G14">
         <v>-1</v>
@@ -1495,8 +1578,8 @@
       <c r="I14">
         <v>-1</v>
       </c>
-      <c r="J14" t="s">
-        <v>117</v>
+      <c r="J14" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1504,22 +1587,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -1527,8 +1610,8 @@
       <c r="I15">
         <v>-1</v>
       </c>
-      <c r="J15" t="s">
-        <v>115</v>
+      <c r="J15" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1536,10 +1619,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1548,7 +1631,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>-1</v>
@@ -1559,8 +1642,8 @@
       <c r="I16">
         <v>-1</v>
       </c>
-      <c r="J16" t="s">
-        <v>116</v>
+      <c r="J16" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1568,16 +1651,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
@@ -1586,13 +1669,13 @@
         <v>-1</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" t="s">
-        <v>118</v>
+        <v>59</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1600,16 +1683,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1">
         <v>4</v>
@@ -1617,14 +1700,14 @@
       <c r="G18">
         <v>-1</v>
       </c>
-      <c r="H18">
-        <v>-1</v>
+      <c r="H18" t="s">
+        <v>21</v>
       </c>
       <c r="I18">
         <v>-1</v>
       </c>
-      <c r="J18" t="s">
-        <v>119</v>
+      <c r="J18" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1635,28 +1718,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1">
         <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19">
-        <v>-1</v>
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>72</v>
       </c>
       <c r="I19" t="s">
-        <v>86</v>
-      </c>
-      <c r="J19" t="s">
-        <v>120</v>
+        <v>72</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1667,28 +1750,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1">
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H20">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" t="s">
-        <v>121</v>
+        <v>73</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1699,13 +1782,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="F21" s="1">
         <v>5</v>
@@ -1719,8 +1802,8 @@
       <c r="I21">
         <v>-1</v>
       </c>
-      <c r="J21" t="s">
-        <v>122</v>
+      <c r="J21" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1731,13 +1814,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F22" s="1">
         <v>6</v>
@@ -1751,8 +1834,8 @@
       <c r="I22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" t="s">
-        <v>123</v>
+      <c r="J22" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1763,19 +1846,19 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1">
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -1783,8 +1866,8 @@
       <c r="I23">
         <v>-1</v>
       </c>
-      <c r="J23" t="s">
-        <v>124</v>
+      <c r="J23" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1795,10 +1878,10 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
         <v>21</v>
@@ -1815,8 +1898,8 @@
       <c r="I24" t="s">
         <v>21</v>
       </c>
-      <c r="J24" t="s">
-        <v>125</v>
+      <c r="J24" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1827,13 +1910,13 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F25" s="1">
         <v>96</v>
@@ -1842,13 +1925,13 @@
         <v>-1</v>
       </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>100</v>
-      </c>
-      <c r="J25" t="s">
-        <v>126</v>
+        <v>85</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1859,13 +1942,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F26" s="1">
         <v>96</v>
@@ -1876,11 +1959,11 @@
       <c r="H26">
         <v>-1</v>
       </c>
-      <c r="I26">
-        <v>-1</v>
-      </c>
-      <c r="J26" t="s">
-        <v>127</v>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1891,13 +1974,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1">
         <v>98</v>
@@ -1911,8 +1994,8 @@
       <c r="I27">
         <v>-1</v>
       </c>
-      <c r="J27" t="s">
-        <v>128</v>
+      <c r="J27" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1923,7 +2006,7 @@
         <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -1955,7 +2038,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D29">
         <v>-1</v>
@@ -1987,7 +2070,7 @@
         <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -2019,7 +2102,7 @@
         <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31">
         <v>-1</v>

</xml_diff>

<commit_message>
Added more synonyms to TextParser.java, including some for nouns. Also cut down on story text to prevent it being cut off in the GUI.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D532639A-B7F6-4AFA-A48B-333D5AA64D40}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5E7B536C-C06F-4C43-A450-7DAEE11FC1B5}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="0" windowWidth="17190" windowHeight="21000" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="17190" yWindow="0" windowWidth="17190" windowHeight="21000" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -304,12 +304,6 @@
     <t>hike</t>
   </si>
   <si>
-    <t>Quest for the Quarantine follows our protagonist, 16-year-old Esperanza, as she navigates post-apocalyptic Mexico in hopes of reaching salvation in the form of the "Quarantine Zone". As we follow Esperanza through her journey, we discover that the most pressing danger is the loss of humanity itself...\n\nWelcome to Quest for the Quarantine! Throughout this playable story you, the player, can enter commands to help Esperanza navigate both her paths and decisions. To begin the game, enter “start game” in the text box below. May you guide Esperanza safely to the Quarantine.</t>
-  </si>
-  <si>
-    <t>In the weeks following The Event, the days were unsafe. She had learned that lesson the hard way with the death of Mama. They took refuge in the night, and for months everything was okay. They even met others who had not succumbed, who were not Violent. They shared stories of past lives, better lives, and hope for salvation. Rumors of a safe zone in the United States, just outside San Diego, persisted among survivors. For a time, they had hope. But slowly, the survivors disappeared, Mama included; so she decided to leave, to seek out the refuge of the quarantine in the States.\n\nShe slipped quietly into the night and made her way through the streets of Mexico City, careful to avoid others. As she approaches the main avenue, she notices a small store along the road heading out of the city. Perhaps I should look for supplies? She ponders. Or is it better to just leave the city?</t>
-  </si>
-  <si>
     <t>The sign above the door reads “Construcentro”. Esperanza steps through the shadowed doorframe and is immediately hit with the smell of mildew. She gazes around the dark store- and notes it’s pretty barren. To her right along the wall is an old storage crate and behind the counter is an unopened delivery box. Outside, some distant shouting appears to grow stronger. If she’s going to grab something, she should be quick.</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
   </si>
   <si>
     <t>It has been nearly two relatively uneventful weeks since Esperanza has departed Mexico City. After roughly 500 km of hiking, her feet hurt, and she is beginning to run low on supplies. On the twelfth day of her journey, she crests a ridge and spots a city in the valley below. Judging by the nearby highway sign, it’s the city of Leon. The sun is beginning to set behind her, and she notes several light sources dotting the city’s landscape- there’s people there, potentially dangerous people. On one hand, she needs to make a supply run, but on the other she really likes being alive. She could possibly give the city a wide berth, ignoring it completely, but only if she has enough water in her backpack.</t>
-  </si>
-  <si>
-    <t>The sun has now fully disappeared behind the horizon as she makes her way into Leon. Old, decrepit cars accentuate the crumbling roadways, abundant with unregulated vegetation. There are definite signs of habitation however, as she notes some uncorroded ammunition shells at the entry of an alleyway. She pauses to look back and reconsider her decision, but eventually decides to continue forward. An hour later she enters a small square overlooking a dry fountain. A dull glow illuminates the city skyline to her right, giving her pause. The time to search is now, she decides, not wanting to risk spending any more time in the city. She gazes around the square and notes a couple potential looting points: an apartment across the square with a shattered second-story window and a fire escape, and a small bodega below with a very rusted wrought-iron door that seems to be barely hanging on. Additionally, she could continue farther down the road.</t>
   </si>
   <si>
     <t>Leon: Bodega</t>
@@ -369,12 +360,6 @@
     <t>The bodega is dimly lit, and it appears to Esperanza that she is far from being the first person to scavenge in here. Empty bottles and wrappers layer the floor. Few things remain untouched. She picks her way around the discarded remnants for a while, but it proves unfruitful. A distant sound, possibly human, cause her to bolt upright, eyes wide. She cocks her head and listens for a while but notices no other sounds. As she makes her way to the doorway, she notices a small cabinet with closed doors behind the counter. It’s low to the ground and otherwise hidden at eye level.</t>
   </si>
   <si>
-    <t>As Esperanza is making her way out of the city, she can’t help but shake the feeling that someone is watching her. She pauses in the dark and searches the shadows for a sign of movement. Nothing. She continues walking, but the process repeats itself at least a dozen more times. And then there’s the noise: a faint jingle, like that of a glass bottle rolling on concrete. Time slows down and she feels every muscle in her body tighten like a loaded spring. She releases and within two steps, the sound of whoops and shouts light up the concrete jungle. She can hear several sets of footsteps behind her in the dark. She sprints- ducking around corners and dodging between cars. After several minutes, she begins to grow tired and the voices more distant. In a dark alley she pauses, catching her breath. It’s make or break time. She estimates that she’s about 5 minutes from the city limits. Can she use something as a distraction perhaps? She thinks she can make the run, but it sure would help to divert their attention. Either way, she needs to get out of the city immediately.</t>
-  </si>
-  <si>
-    <t>A week later, Esperanza finds herself trudging along a dirt road in the midday heat. A nearby sign points back the way she came and reads “El Chayote – 20 km”. Since Leon, she had played it safe and avoided any large settlements. No need to press my luck, she thinks to herself. As she comes around a bend in the road, she notices a small farmstead to her right. The remnants of a fenced pasture dot the roadside, but there is no livestock to be seen. A small dirt path winds from the road back several hundred meters to a house. At the end of the path is a wooden chair, and in that chair, an elderly man. He nods to Esperanza as she approaches, and she regards him cautiously. After some small discussion, the farmer attempts to initiate a barter. He wants any ammunition she may have and he’s offering the contents of a medium-sized sack he has laying on the ground next to his chair and a small, wooden box.</t>
-  </si>
-  <si>
     <t>Quest for the Quarantine</t>
   </si>
   <si>
@@ -440,8 +425,62 @@
     <t>The fear is too great, and rightly so. She turns and quickly tiptoes back out of the window and down the fire escape.</t>
   </si>
   <si>
+    <t>She pulls open the cabinet doors and hurriedly searches, grasping a bottle of water and a small packet of food. Good enough for me, she concludes, before turning and leaving the store.</t>
+  </si>
+  <si>
+    <t>The sound has her spooked and she decides to just get away from the square with haste. She steps out of the store and keeps winding her way through the rubble and down the street.</t>
+  </si>
+  <si>
+    <t>Pulling the firecrackers out of her pocket, she quickly lights them and lobs them over the roof of the building behind her. She pivots 180 degrees and immediately sprints down the roadway. Behind her the sounds of cracks, snaps, and pops greet her, followed by a delayed shouting. She grins assuredly (success!) and is out of the city limits within a few minutes.</t>
+  </si>
+  <si>
+    <t>Mistakenly she immediately runs out of the alley and into a shadowy figure, both falling to the ground. She scrambles to her feet, but the person has a hand on her backpack. Digging her heels in, she pulls forward and a small ripping sound issues from her backpack. The person falls to the ground again and the sound of something falling out of her backpack fills the night. No time. She sprints with every ounce of energy she can muster and is out of the city in minutes, alone and safe.</t>
+  </si>
+  <si>
+    <t>Esperanza acquiesces and holds out her ammo. The farmer looks excited and hands her the sack in return, which she then opens and peers inside. The contents are a small first aid kit and a cooking pan; they could prove useful. She throws the sack over her shoulder, waves goodbye, and continues down the dirt road.</t>
+  </si>
+  <si>
+    <t>She politely declines the farmer’s offer and wishes him well. It’s a relief to meet someone not Violent, she thinks to herself as she continues down the dirt road. Something that seems to be happening less frequently as time wears on.</t>
+  </si>
+  <si>
+    <t>As Esperanza’s odyssey continues, the mountains in the distance continue to grow larger. She knows the time is getting near for her to traverse the range and reach the western side. As she reaches the foothills, a small village lies in her path. At first observation, it seems completely abandoned. This might be her last chance to get supplies before she summits, but it isn’t devoid of risk. She would need water if she were going to go around the town.</t>
+  </si>
+  <si>
+    <t>pocketknife,water</t>
+  </si>
+  <si>
+    <t>She has water to spare and no time to waste, so she gives the village a wide berth and continues on her way.</t>
+  </si>
+  <si>
+    <t>She walks down the small main road and into the village. The place is devoid of any signs of life, a sadly reassuring attribute to Esperanza. Towards the center of the village, she finds an overturned truck with its contents and broken glass strewn about. She rummages about and is able to acquire a pocketknife in quite good condition and another bottle of water. Satisfied, she follows the road out of the village.</t>
+  </si>
+  <si>
+    <t>Hydrate or die-drate, she muses. She downs another liter of water, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>A rumbling stomach concludes that she needs to eat. She downs another packet of food, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>Using her machete, she’s able to turn a roaming tortoise into a solid meal. She eats, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
+  </si>
+  <si>
+    <t>Ambitiously, she immediately begins the hike into the mountains. Within hours she feels extremely weak and can barely move. Her muscles tighten and cramp with every passing moment. Her breath gets harder to catch, the panting is never-ending. Her vision slowly begins to fade, but not before she notices several moving shapes around her. Coyotes are circling her. A sharp pain followed by warmth. And then darkness.</t>
+  </si>
+  <si>
+    <t>Quest for the Quarantine follows our protagonist, 16-year-old Esperanza, as she navigates post-apocalyptic Mexico in hopes of reaching salvation in the form of the "Quarantine Zone". As we follow Esperanza through her journey, we discover that the most pressing danger is the loss of humanity itself... Welcome to Quest for the Quarantine! Throughout this playable story you, the player, can enter commands to help Esperanza navigate both her paths and decisions. Commands must be in the form of “verb noun”. To begin the game, enter “start game” in the text box below. May you guide Esperanza safely to the Quarantine.</t>
+  </si>
+  <si>
+    <t>In the weeks following The Event, the days were unsafe. She had learned that lesson the hard way with the death of Mama. They took refuge in the night, and for months everything was okay. They even met others who had not succumbed, who were not Violent. They shared stories of past lives, better lives, and hope for salvation. Rumors of a safe zone in the United States, just outside San Diego, persisted among survivors. For a time, they had hope. But slowly, the survivors disappeared, Mama included; so she decided to leave, to seek out the refuge of the quarantine in the States. She slipped quietly into the night and made her way through the streets of Mexico City, careful to avoid others. As she approaches the main avenue, she notices a small store along the road heading out of the city. Perhaps I should look for supplies? She ponders. Or is it better to just leave the city?</t>
+  </si>
+  <si>
+    <t>The sun has now fully disappeared behind the horizon as she makes her way into Leon. Old, decrepit cars accentuate the crumbling roadways, abundant with unregulated vegetation. There are definite signs of habitation however, as she notes some uncorroded ammunition shells at the entry of an alleyway. She pauses to look back and reconsider her decision, but eventually decides to continue forward. An hour later she enters a small square overlooking a dry fountain. A dull glow illuminates the city skyline to her right, giving her pause. She gazes around the square and notes a couple potential looting points: an apartment across the square with a shattered second-story window and a fire escape, and a small bodega below with a very rusted wrought-iron door that seems to be barely hanging on. Additionally, she could continue farther down the road.</t>
+  </si>
+  <si>
+    <t>As Esperanza is making her way out of the city, she can’t help but shake the feeling that someone is watching her. She pauses in the dark and searches the shadows for a sign of movement. Nothing. And then there’s noise: a faint jingle, like that of a glass bottle rolling on concrete. Time slows down and she feels every muscle in her body tighten like a loaded spring. She releases and within two steps, the sound of whoops and shouts light up the concrete jungle. She can hear several sets of footsteps in pursuit. She sprints- ducking around corners and dodging between cars. Minutes later in a dark alley she pauses, catching her breath. Can she use something as a distraction perhaps? She thinks she can make it out of the city, but it sure would help to divert their attention.</t>
+  </si>
+  <si>
     <r>
-      <t>Risk versus reward…. the potential reward is quite tempting. Taking a deep breath, she steps into the bedroom and begins searching. The last place she checks is under the bed: a small wooden keepsake box resides there. She opens it and her eyes grow wide at the sight of some pistol ammunition and a string of firecrackers. Excitedly she shoves them in her pockets and rushes out of the room. A previously unseen wet spot causes her to slip and fall backwards into the closed door, forcing it open. She lands on her butt with her back against a solid piece of furniture. The smell is overwhelming now, and she immediately squints her eyes and vomits. Sitting back up, she notices a faint brushing against her cheek. She is paralyzed in fear but manages to look out of the corner of her eye. Toes</t>
+      <t>Taking a deep breath, she steps into the bedroom. The last place she checks is under the bed: a small wooden keepsake box resides there. She opens it and her eyes grow wide at the sight of some pistol ammunition and a string of firecrackers. Excitedly she shoves them in her pockets and rushes out of the room. A previously unseen wet spot causes her to slip and fall backwards into the closed door, forcing it open. The smell is overwhelming now, and she immediately squints her eyes and vomits. Sitting back up, she notices a faint brushing against her cheek. She is paralyzed in fear but manages to look out of the corner of her eye. Toes</t>
     </r>
     <r>
       <rPr>
@@ -462,62 +501,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> are rubbing against her cheek, suspended from above. Not daring to look up, she crawls on all fours out of the new room and scrambles to get out of the apartment and out of this city.</t>
+      <t xml:space="preserve"> are rubbing against her cheek, suspended from above. Not daring to look up, she crawls on all fours out of the new room and scrambles out of the apartment.</t>
     </r>
   </si>
   <si>
-    <t>She pulls open the cabinet doors and hurriedly searches, grasping a bottle of water and a small packet of food. Good enough for me, she concludes, before turning and leaving the store.</t>
-  </si>
-  <si>
-    <t>The sound has her spooked and she decides to just get away from the square with haste. She steps out of the store and keeps winding her way through the rubble and down the street.</t>
-  </si>
-  <si>
-    <t>Pulling the firecrackers out of her pocket, she quickly lights them and lobs them over the roof of the building behind her. She pivots 180 degrees and immediately sprints down the roadway. Behind her the sounds of cracks, snaps, and pops greet her, followed by a delayed shouting. She grins assuredly (success!) and is out of the city limits within a few minutes.</t>
-  </si>
-  <si>
-    <t>Mistakenly she immediately runs out of the alley and into a shadowy figure, both falling to the ground. She scrambles to her feet, but the person has a hand on her backpack. Digging her heels in, she pulls forward and a small ripping sound issues from her backpack. The person falls to the ground again and the sound of something falling out of her backpack fills the night. No time. She sprints with every ounce of energy she can muster and is out of the city in minutes, alone and safe.</t>
-  </si>
-  <si>
-    <t>Esperanza acquiesces and holds out her ammo. The farmer looks excited and hands her the sack in return, which she then opens and peers inside. The contents are a small first aid kit and a cooking pan; they could prove useful. She throws the sack over her shoulder, waves goodbye, and continues down the dirt road.</t>
-  </si>
-  <si>
-    <t>Esperanza whips out her machete and raises it in the air menacingly. Surprised, the farmer stumbles backwards, a look of betrayal in his eyes. She tells him to run and he doesn’t hesitate, bounding back towards the house with the sack in his hand. She readies to follow him but notices the wooden box on the ground. Opening it, she finds a pistol and some food. Deciding that’s enough of a procurement, she let’s the farmer live another day.</t>
-  </si>
-  <si>
-    <t>She politely declines the farmer’s offer and wishes him well. It’s a relief to meet someone not Violent, she thinks to herself as she continues down the dirt road. Something that seems to be happening less frequently as time wears on.</t>
-  </si>
-  <si>
-    <t>As Esperanza’s odyssey continues, the mountains in the distance continue to grow larger. She knows the time is getting near for her to traverse the range and reach the western side. As she reaches the foothills, a small village lies in her path. At first observation, it seems completely abandoned. This might be her last chance to get supplies before she summits, but it isn’t devoid of risk. She would need water if she were going to go around the town.</t>
-  </si>
-  <si>
-    <t>pocketknife,water</t>
-  </si>
-  <si>
-    <t>She has water to spare and no time to waste, so she gives the village a wide berth and continues on her way.</t>
-  </si>
-  <si>
-    <t>She walks down the small main road and into the village. The place is devoid of any signs of life, a sadly reassuring attribute to Esperanza. Towards the center of the village, she finds an overturned truck with its contents and broken glass strewn about. She rummages about and is able to acquire a pocketknife in quite good condition and another bottle of water. Satisfied, she follows the road out of the village.</t>
-  </si>
-  <si>
-    <t>Hydrate or die-drate, she muses. She downs another liter of water, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
-  </si>
-  <si>
-    <t>A rumbling stomach concludes that she needs to eat. She downs another packet of food, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
-  </si>
-  <si>
-    <t>Using her machete, she’s able to turn a roaming tortoise into a solid meal. She eats, takes a quick nap, and then begins to pack up camp. After some quick stretching, she sighs and looks to the valley behind her. Expanding far to the south, she squints as her eyes gaze over it. Somewhere down there is her home. Or what used to be her home. She shakes off the melancholy, shoulders her backpack higher, and steps off into the mountains, never again looking back.</t>
-  </si>
-  <si>
-    <t>Ambitiously, she immediately begins the hike into the mountains. Within hours she feels extremely weak and can barely move. Her muscles tighten and cramp with every passing moment. Her breath gets harder to catch, the panting is never-ending. Her vision slowly begins to fade, but not before she notices several moving shapes around her. Coyotes are circling her. A sharp pain followed by warmth. And then darkness.</t>
+    <t>A week later, Esperanza finds herself trudging along a dirt road in the midday heat. A nearby sign points back the way she came and reads “El Chayote – 20 km”. Since Leon, she had played it safe and avoided any large settlements. As she comes around a bend in the road, she notices a small farmstead to her right. The remnants of a fenced pasture dot the roadside, but there is no livestock to be seen. A small dirt path winds from the road back several hundred meters to a house. At the end of the path is a wooden chair, and in that chair, an elderly man. He nods to Esperanza as she approaches, and she regards him cautiously. After some small discussion, the farmer attempts to initiate a barter. He wants  ammo and he’s offering the contents of a medium-sized sack he has laying on the ground next to his chair.</t>
+  </si>
+  <si>
+    <t>Esperanza whips out her machete and raises it in the air menacingly. Surprised, the farmer stumbles backwards, a look of betrayal in his eyes. She tells him to run and he doesn’t hesitate, bounding back towards the house with the sack in his hand. She readies to follow him but notices a wooden box on the ground under the chair. Opening it, she finds a pistol and some food. Deciding that’s enough of a procurement, she let’s the farmer live another day.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -593,15 +600,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -927,7 +937,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -953,10 +963,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,10 +985,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +999,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,8 +1009,8 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>98</v>
+      <c r="C6" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,8 +1020,8 @@
       <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>100</v>
+      <c r="C7" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1019,10 +1029,10 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1032,8 +1042,8 @@
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>103</v>
+      <c r="C9" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1043,8 +1053,8 @@
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>104</v>
+      <c r="C10" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,7 +1065,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1087,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,7 +1098,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1109,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
@@ -1110,11 +1120,11 @@
         <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1125,7 +1135,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1237,7 @@
         <v>-1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1259,7 +1269,7 @@
         <v>-1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1270,13 +1280,13 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1291,7 +1301,7 @@
         <v>-1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1302,13 +1312,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1323,7 +1333,7 @@
         <v>-1</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1355,7 +1365,7 @@
         <v>-1</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1387,7 +1397,7 @@
         <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1419,7 +1429,7 @@
         <v>-1</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1451,7 +1461,7 @@
         <v>-1</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1468,7 +1478,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>36</v>
@@ -1483,7 +1493,7 @@
         <v>-1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1515,7 +1525,7 @@
         <v>-1</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1546,8 +1556,8 @@
       <c r="I13">
         <v>-1</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>123</v>
+      <c r="J13" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1579,7 +1589,7 @@
         <v>-1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1611,7 +1621,7 @@
         <v>-1</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1643,7 +1653,7 @@
         <v>-1</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1675,7 +1685,7 @@
         <v>59</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1707,7 +1717,7 @@
         <v>-1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1739,7 +1749,7 @@
         <v>72</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1770,8 +1780,8 @@
       <c r="I20" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>129</v>
+      <c r="J20" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1803,7 +1813,7 @@
         <v>-1</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1835,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1858,7 +1868,7 @@
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -1867,7 +1877,7 @@
         <v>-1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1899,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1931,7 +1941,7 @@
         <v>85</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1963,7 +1973,7 @@
         <v>73</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1995,7 +2005,7 @@
         <v>-1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made options for Leon:Alleway more explicit. Shortened string in Viewer.java.
</commit_message>
<xml_diff>
--- a/quarantine_first_edition.xlsx
+++ b/quarantine_first_edition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/096e9b8dd598cc03/Documents/Quarantine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5E7B536C-C06F-4C43-A450-7DAEE11FC1B5}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{34A1259C-05FE-F043-84AA-4763E9495BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{90C8289F-12CA-48C9-8F23-914E2BAE4DA8}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="0" windowWidth="17190" windowHeight="21000" activeTab="1" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
+    <workbookView xWindow="17190" yWindow="0" windowWidth="17190" windowHeight="21000" xr2:uid="{1A8EC298-E68E-6745-816B-800EA509D514}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -476,9 +476,6 @@
     <t>The sun has now fully disappeared behind the horizon as she makes her way into Leon. Old, decrepit cars accentuate the crumbling roadways, abundant with unregulated vegetation. There are definite signs of habitation however, as she notes some uncorroded ammunition shells at the entry of an alleyway. She pauses to look back and reconsider her decision, but eventually decides to continue forward. An hour later she enters a small square overlooking a dry fountain. A dull glow illuminates the city skyline to her right, giving her pause. She gazes around the square and notes a couple potential looting points: an apartment across the square with a shattered second-story window and a fire escape, and a small bodega below with a very rusted wrought-iron door that seems to be barely hanging on. Additionally, she could continue farther down the road.</t>
   </si>
   <si>
-    <t>As Esperanza is making her way out of the city, she can’t help but shake the feeling that someone is watching her. She pauses in the dark and searches the shadows for a sign of movement. Nothing. And then there’s noise: a faint jingle, like that of a glass bottle rolling on concrete. Time slows down and she feels every muscle in her body tighten like a loaded spring. She releases and within two steps, the sound of whoops and shouts light up the concrete jungle. She can hear several sets of footsteps in pursuit. She sprints- ducking around corners and dodging between cars. Minutes later in a dark alley she pauses, catching her breath. Can she use something as a distraction perhaps? She thinks she can make it out of the city, but it sure would help to divert their attention.</t>
-  </si>
-  <si>
     <r>
       <t>Taking a deep breath, she steps into the bedroom. The last place she checks is under the bed: a small wooden keepsake box resides there. She opens it and her eyes grow wide at the sight of some pistol ammunition and a string of firecrackers. Excitedly she shoves them in her pockets and rushes out of the room. A previously unseen wet spot causes her to slip and fall backwards into the closed door, forcing it open. The smell is overwhelming now, and she immediately squints her eyes and vomits. Sitting back up, she notices a faint brushing against her cheek. She is paralyzed in fear but manages to look out of the corner of her eye. Toes</t>
     </r>
@@ -510,14 +507,24 @@
   <si>
     <t>Esperanza whips out her machete and raises it in the air menacingly. Surprised, the farmer stumbles backwards, a look of betrayal in his eyes. She tells him to run and he doesn’t hesitate, bounding back towards the house with the sack in his hand. She readies to follow him but notices a wooden box on the ground under the chair. Opening it, she finds a pistol and some food. Deciding that’s enough of a procurement, she let’s the farmer live another day.</t>
   </si>
+  <si>
+    <t>As Esperanza is making her way out of the city, she can’t help but shake the feeling that someone is watching her. She pauses in the dark and searches the shadows for a sign of movement. Nothing. And then there’s noise: a faint jingle, like that of a glass bottle rolling on concrete. Time slows down and she feels every muscle in her body tighten like a loaded spring. She releases and within two steps, the sound of whoops and shouts light up the concrete jungle. She can hear several sets of footsteps in pursuit. She sprints- ducking around corners and dodging between cars. Minutes later in a dark alley she pauses, catching her breath. Can she use something as a distraction perhaps? She thinks she can make a run for it regardless, but it sure would help to divert their attention.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -600,15 +607,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -936,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BB1A2F-63DD-CA4F-86FF-FB6F4E825AE5}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1042,8 +1052,8 @@
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>135</v>
+      <c r="C9" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,7 +1064,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,7 +1134,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1134,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA4819E-E7B0-F54E-83C6-1AB902CEB676}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -1557,7 +1567,7 @@
         <v>-1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1781,7 +1791,7 @@
         <v>73</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>